<commit_message>
fix new bus relation type
</commit_message>
<xml_diff>
--- a/bin/resource/excel/meta_class.xlsx
+++ b/bin/resource/excel/meta_class.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opensource\ark_new\bin\resource\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FC1EEB-F2B1-4570-B0E0-9C274E5A08EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="27870" windowHeight="13065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -14,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>1</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="111">
   <si>
     <t>class</t>
   </si>
@@ -373,19 +379,21 @@
   </si>
   <si>
     <t>最大魔法值</t>
+  </si>
+  <si>
+    <t>log</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>改变时log</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,163 +415,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.35"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.35"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,198 +473,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.25"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -798,255 +501,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1065,62 +526,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1378,19 +801,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.25" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
@@ -1403,9 +826,10 @@
     <col min="13" max="13" width="10.375" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="10.875" customWidth="1"/>
+    <col min="16" max="16" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1451,8 +875,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" s="2" customFormat="1" spans="1:15">
+      <c r="P1" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1498,8 +925,11 @@
       <c r="O2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1526,8 +956,11 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-    </row>
-    <row r="4" customFormat="1" spans="1:20">
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1557,13 +990,15 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="3"/>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1593,13 +1028,15 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="3"/>
+      <c r="P5">
+        <v>0</v>
+      </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1626,8 +1063,11 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1654,8 +1094,11 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1682,8 +1125,11 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1710,8 +1156,11 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1738,8 +1187,11 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1766,8 +1218,11 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1794,8 +1249,11 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1822,8 +1280,11 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1850,8 +1311,11 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1878,8 +1342,11 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1906,8 +1373,11 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1934,8 +1404,11 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1962,8 +1435,11 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1990,8 +1466,11 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2018,8 +1497,11 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2046,8 +1528,11 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2074,8 +1559,11 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2089,7 +1577,6 @@
         <v>76</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23"/>
       <c r="G23" t="s">
         <v>77</v>
       </c>
@@ -2106,8 +1593,11 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2137,8 +1627,11 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2168,8 +1661,11 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2196,8 +1692,11 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2224,8 +1723,11 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2252,8 +1754,11 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -2280,8 +1785,11 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2308,8 +1816,11 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>81</v>
       </c>
@@ -2336,8 +1847,11 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2364,8 +1878,11 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -2392,8 +1909,11 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2420,8 +1940,11 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2448,8 +1971,11 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -2476,8 +2002,11 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>77</v>
       </c>
@@ -2504,10 +2033,14 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
+      <c r="P37">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>